<commit_message>
EPBDS-2753 Fix Dispatching Method test source. Added test for duplicate datatypes in dependencies.
</commit_message>
<xml_diff>
--- a/STUDIO/trunk/org.openl.rules.project/test/resources/dependencies/testMethodDispatching/dependency-module/dependencyModule1.xlsx
+++ b/STUDIO/trunk/org.openl.rules.project/test/resources/dependencies/testMethodDispatching/dependency-module/dependencyModule1.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Rules String hello1(int hour)</t>
   </si>
@@ -67,13 +65,22 @@
   </si>
   <si>
     <t>Good Night</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>lob</t>
+  </si>
+  <si>
+    <t>lob2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,8 +104,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +141,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -395,6 +413,21 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -404,11 +437,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
@@ -430,6 +460,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -437,6 +473,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -515,6 +556,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -549,6 +591,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -724,112 +767,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D7:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D7:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
     <col min="6" max="6" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:6">
-      <c r="D7" s="1" t="s">
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="4:6" ht="15.75" thickBot="1">
-      <c r="D8" s="20" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="4:6">
-      <c r="D9" s="6" t="s">
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="4:6" ht="15.75" thickBot="1">
-      <c r="D10" s="3" t="s">
+    <row r="11" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="4:6" ht="15.75" thickBot="1">
-      <c r="D11" s="8" t="s">
+    <row r="12" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="4:6">
-      <c r="D12" s="10">
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="9">
         <v>0</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E13" s="10">
         <v>11</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="4:6">
-      <c r="D13" s="12">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="11">
         <v>12</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E14" s="12">
         <v>17</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F14" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="4:6">
-      <c r="D14" s="12">
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="11">
         <v>18</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E15" s="12">
         <v>21</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="4:6" ht="15.75" thickBot="1">
-      <c r="D15" s="14">
+    <row r="16" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="13">
         <v>22</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E16" s="14">
         <v>23</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F16" s="18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -838,29 +892,6 @@
     <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>